<commit_message>
ya en prod admisiones
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$K$44</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -204,7 +207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +244,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -544,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -585,6 +596,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -702,21 +735,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -729,38 +762,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1076,37 +1088,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
     </row>
     <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1129,300 +1142,300 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74" t="s">
+      <c r="D5" s="80"/>
+      <c r="E5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74" t="s">
+      <c r="F5" s="80"/>
+      <c r="G5" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74" t="s">
+      <c r="H5" s="80"/>
+      <c r="I5" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="81"/>
     </row>
     <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="49"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45" t="s">
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45" t="s">
+      <c r="E7" s="53"/>
+      <c r="F7" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45" t="s">
+      <c r="G7" s="53"/>
+      <c r="H7" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45" t="s">
+      <c r="I7" s="53"/>
+      <c r="J7" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="46"/>
+      <c r="K7" s="54"/>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="49"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45" t="s">
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45" t="s">
+      <c r="E9" s="53"/>
+      <c r="F9" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45" t="s">
+      <c r="G9" s="53"/>
+      <c r="H9" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="45"/>
-      <c r="J9" s="66" t="s">
+      <c r="I9" s="53"/>
+      <c r="J9" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="67"/>
+      <c r="K9" s="73"/>
     </row>
     <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="49"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="65" t="s">
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="69"/>
-      <c r="H11" s="65" t="s">
+      <c r="G11" s="77"/>
+      <c r="H11" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="69"/>
-      <c r="J11" s="66" t="s">
+      <c r="I11" s="77"/>
+      <c r="J11" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="67"/>
+      <c r="K11" s="73"/>
     </row>
     <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="49"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="65" t="s">
+      <c r="B13" s="72"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="69"/>
-      <c r="F13" s="65" t="s">
+      <c r="E13" s="77"/>
+      <c r="F13" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="69"/>
-      <c r="H13" s="66" t="s">
+      <c r="G13" s="77"/>
+      <c r="H13" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="67"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="73"/>
     </row>
     <row r="14" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="49"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="65" t="s">
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="73"/>
     </row>
     <row r="16" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="49"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="80"/>
-    </row>
-    <row r="18" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
-      <c r="K18" s="82"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="59" t="s">
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="28"/>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="63" t="s">
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="64"/>
-      <c r="H19" s="63" t="s">
+      <c r="G19" s="75"/>
+      <c r="H19" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="64"/>
-      <c r="J19" s="45" t="s">
+      <c r="I19" s="75"/>
+      <c r="J19" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="46"/>
-    </row>
-    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="49"/>
-    </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="59" t="s">
+      <c r="K19" s="54"/>
+    </row>
+    <row r="20" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="55"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="57"/>
+    </row>
+    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60" t="s">
+      <c r="B21" s="68"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="61"/>
-    </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="69"/>
+    </row>
+    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="52"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1430,103 +1443,103 @@
       <c r="J22" s="3"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+    <row r="23" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="51"/>
+      <c r="B23" s="59"/>
       <c r="C23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="52" t="s">
+      <c r="D23" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="53"/>
+      <c r="E23" s="61"/>
       <c r="F23" s="6" t="s">
         <v>35</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="53"/>
-      <c r="J23" s="55" t="s">
+      <c r="I23" s="61"/>
+      <c r="J23" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="56"/>
-    </row>
-    <row r="24" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="48"/>
+      <c r="K23" s="64"/>
+    </row>
+    <row r="24" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="49"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="D24" s="56"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="57"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="43"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="46"/>
-    </row>
-    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="49"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="51"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="52"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="54"/>
+    </row>
+    <row r="27" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="55"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="57"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="34" t="s">
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="K28" s="35"/>
-    </row>
-    <row r="29" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="43"/>
+    </row>
+    <row r="29" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -1539,7 +1552,7 @@
       <c r="J29" s="12"/>
       <c r="K29" s="13"/>
     </row>
-    <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1552,21 +1565,25 @@
       <c r="J30" s="12"/>
       <c r="K30" s="13"/>
     </row>
-    <row r="31" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="13"/>
-    </row>
-    <row r="32" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="39"/>
+    </row>
+    <row r="32" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1577,9 +1594,8 @@
       <c r="I32" s="11"/>
       <c r="J32" s="12"/>
       <c r="K32" s="13"/>
-      <c r="M32" s="14"/>
-    </row>
-    <row r="33" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -1592,269 +1608,214 @@
       <c r="J33" s="12"/>
       <c r="K33" s="13"/>
     </row>
-    <row r="34" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="K34" s="31"/>
-    </row>
-    <row r="35" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="13"/>
-    </row>
-    <row r="36" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="11"/>
+    <row r="34" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="14"/>
+    </row>
+    <row r="35" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" s="39"/>
+    </row>
+    <row r="36" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="17"/>
       <c r="J36" s="12"/>
       <c r="K36" s="13"/>
     </row>
-    <row r="37" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="12"/>
+    <row r="37" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="18"/>
       <c r="K37" s="13"/>
-      <c r="L37" s="14"/>
-    </row>
-    <row r="38" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="K38" s="31"/>
-    </row>
-    <row r="39" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="13"/>
-    </row>
-    <row r="40" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="13"/>
-    </row>
-    <row r="41" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="13"/>
-    </row>
-    <row r="42" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="N37" s="31"/>
+    </row>
+    <row r="38" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B38" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C38" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20" t="s">
+      <c r="D38" s="20"/>
+      <c r="E38" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20" t="s">
+      <c r="F38" s="20"/>
+      <c r="G38" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="32" t="s">
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K42" s="33"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="22" t="s">
+      <c r="K38" s="41"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C39" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22" t="s">
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="34" t="s">
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="J43" s="34"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="43"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="44"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="46"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="14"/>
+    </row>
+    <row r="42" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="14"/>
+    </row>
+    <row r="43" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
       <c r="K43" s="35"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="38"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="22" t="s">
-        <v>55</v>
-      </c>
+      <c r="L43" s="14"/>
+    </row>
+    <row r="44" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L44" s="14"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="14"/>
-    </row>
-    <row r="46" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="14"/>
-    </row>
-    <row r="47" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="14"/>
-    </row>
-    <row r="48" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L48" s="14"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="85">
@@ -1874,22 +1835,16 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:K10"/>
@@ -1897,6 +1852,12 @@
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
@@ -1933,17 +1894,18 @@
     <mergeCell ref="A26:K27"/>
     <mergeCell ref="A28:I28"/>
     <mergeCell ref="J28:K28"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A46:K46"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="J35:K35"/>
     <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="A41:G41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>